<commit_message>
Changing and deleting files
</commit_message>
<xml_diff>
--- a/DRP/demand_data_2suppliers.xlsx
+++ b/DRP/demand_data_2suppliers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE80BACC-4435-477F-B167-4C8D359B341B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2165EC-4994-48BB-BF91-FB12C54B6749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC1" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="162">
   <si>
     <t>W46</t>
   </si>
@@ -829,6 +829,9 @@
   </si>
   <si>
     <t>Spot Demand to reduce (lotsize)</t>
+  </si>
+  <si>
+    <t>truck availaibity</t>
   </si>
 </sst>
 </file>
@@ -5221,50 +5224,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1028699</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>43004</xdr:colOff>
-      <xdr:row>158</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EE9BF40-2472-44FA-AC7E-873BB71C06FB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14714219" y="27043380"/>
-          <a:ext cx="10040445" cy="2202180"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5534,7 +5493,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5792,19 +5751,19 @@
         <v>30</v>
       </c>
       <c r="F13" s="11">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G13" s="11">
+        <v>15</v>
+      </c>
+      <c r="H13" s="11">
+        <v>50</v>
+      </c>
+      <c r="I13" s="11">
         <v>20</v>
       </c>
-      <c r="H13" s="11">
+      <c r="J13" s="11">
         <v>100</v>
-      </c>
-      <c r="I13" s="11">
-        <v>70</v>
-      </c>
-      <c r="J13" s="11">
-        <v>0</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="12">
@@ -5974,7 +5933,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6228,7 +6187,7 @@
       </c>
       <c r="C13" s="223"/>
       <c r="D13" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11">
@@ -6238,13 +6197,13 @@
         <v>20</v>
       </c>
       <c r="H13" s="11">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I13" s="11">
+        <v>25</v>
+      </c>
+      <c r="J13" s="11">
         <v>60</v>
-      </c>
-      <c r="J13" s="11">
-        <v>100</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="12">
@@ -6408,7 +6367,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6673,7 +6632,9 @@
       <c r="G13" s="210">
         <v>10</v>
       </c>
-      <c r="H13" s="210"/>
+      <c r="H13" s="210">
+        <v>45</v>
+      </c>
       <c r="I13" s="210">
         <v>100</v>
       </c>
@@ -6845,10 +6806,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF45C3FC-159B-4BF0-B980-4093E4D988CE}">
-  <dimension ref="B2:M11"/>
+  <dimension ref="B2:M16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6880,7 +6841,7 @@
       </c>
       <c r="C4" s="42">
         <f>C6*C7</f>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>25</v>
@@ -6917,7 +6878,7 @@
         <v>150</v>
       </c>
       <c r="C6" s="39">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D6" s="4"/>
       <c r="G6" s="4"/>
@@ -6932,7 +6893,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="43">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -6980,7 +6941,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -6998,6 +6959,11 @@
       </c>
       <c r="H11" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -7030,7 +6996,7 @@
   <dimension ref="B2:M11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7062,7 +7028,7 @@
       </c>
       <c r="C4" s="42">
         <f>C6*C7</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>25</v>
@@ -7099,7 +7065,7 @@
         <v>150</v>
       </c>
       <c r="C6" s="39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4"/>
       <c r="G6" s="4"/>
@@ -7440,23 +7406,23 @@
       </c>
       <c r="J14" s="245">
         <f>'DC1'!F13</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="K14" s="248">
         <f>'DC1'!G13</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L14" s="245">
         <f>'DC1'!H13</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M14" s="245">
         <f>'DC1'!I13</f>
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="N14" s="245">
         <f>'DC1'!J13</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O14" s="245">
         <f>'DC1'!K13</f>
@@ -7633,23 +7599,23 @@
       </c>
       <c r="J18" s="61">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="K18" s="61">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L18" s="61">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M18" s="61">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="N18" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O18" s="61">
         <f t="shared" si="0"/>
@@ -7707,7 +7673,7 @@
       </c>
       <c r="J20" s="68">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K20" s="68">
         <f t="shared" si="1"/>
@@ -7759,23 +7725,23 @@
       </c>
       <c r="J21" s="68">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="K21" s="68">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L21" s="68">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M21" s="68">
         <f t="shared" si="2"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="N21" s="68">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O21" s="68">
         <f t="shared" si="2"/>
@@ -7808,23 +7774,23 @@
       </c>
       <c r="J22" s="68">
         <f t="shared" ref="J22:P22" si="4" xml:space="preserve"> CEILING(J21/$F$11,1)*$F$11</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="K22" s="68">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L22" s="68">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M22" s="68">
         <f t="shared" si="4"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="N22" s="68">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O22" s="68">
         <f t="shared" si="4"/>
@@ -7846,23 +7812,23 @@
       </c>
       <c r="H23" s="75">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I23" s="75">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="J23" s="75">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K23" s="75">
         <f t="shared" si="5"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="L23" s="75">
         <f>N22</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M23" s="75">
         <f t="shared" ref="M23:P23" si="6">O22</f>
@@ -7896,15 +7862,15 @@
       </c>
       <c r="I24" s="79">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="79">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="79">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="79">
         <f t="shared" si="7"/>
@@ -7939,23 +7905,23 @@
       </c>
       <c r="H25" s="83">
         <f t="shared" ref="H25:P25" si="8">QUOTIENT(H23+$F$6-1,$F$5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I25" s="83">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J25" s="83">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K25" s="83">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L25" s="83">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M25" s="83">
         <f t="shared" si="8"/>
@@ -7985,23 +7951,23 @@
       </c>
       <c r="H26" s="87">
         <f t="shared" ref="H26:P26" si="9">IF($Q$26="Choosing Supplier 1", H25*$G$5+H24*$G$6,H25*$G$7+H24*$G$8)</f>
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="I26" s="87">
         <f t="shared" si="9"/>
-        <v>2400</v>
+        <v>2150</v>
       </c>
       <c r="J26" s="87">
         <f t="shared" si="9"/>
-        <v>3000</v>
+        <v>1550</v>
       </c>
       <c r="K26" s="87">
         <f t="shared" si="9"/>
-        <v>3350</v>
+        <v>1800</v>
       </c>
       <c r="L26" s="87">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="M26" s="87">
         <f t="shared" si="9"/>
@@ -8087,23 +8053,23 @@
       </c>
       <c r="H28" s="96">
         <f>H27*H23</f>
-        <v>16880</v>
+        <v>12660</v>
       </c>
       <c r="I28" s="96">
         <f t="shared" si="10"/>
-        <v>17040</v>
+        <v>14910</v>
       </c>
       <c r="J28" s="96">
         <f t="shared" si="10"/>
-        <v>21500</v>
+        <v>10750</v>
       </c>
       <c r="K28" s="96">
         <f t="shared" si="10"/>
-        <v>23650</v>
+        <v>12900</v>
       </c>
       <c r="L28" s="96">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>21600</v>
       </c>
       <c r="M28" s="96">
         <f t="shared" si="10"/>
@@ -8139,23 +8105,23 @@
       </c>
       <c r="H29" s="100">
         <f t="shared" si="11"/>
-        <v>19280</v>
+        <v>14460</v>
       </c>
       <c r="I29" s="100">
         <f t="shared" si="11"/>
-        <v>19440</v>
+        <v>17060</v>
       </c>
       <c r="J29" s="100">
         <f t="shared" si="11"/>
-        <v>24500</v>
+        <v>12300</v>
       </c>
       <c r="K29" s="100">
         <f t="shared" si="11"/>
-        <v>27000</v>
+        <v>14700</v>
       </c>
       <c r="L29" s="100">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>24600</v>
       </c>
       <c r="M29" s="100">
         <f t="shared" si="11"/>
@@ -8237,23 +8203,23 @@
       </c>
       <c r="H31" s="104">
         <f t="shared" ref="H31:P31" si="12">H30*H23</f>
-        <v>33040</v>
+        <v>24780</v>
       </c>
       <c r="I31" s="104">
         <f t="shared" si="12"/>
-        <v>32800</v>
+        <v>28700</v>
       </c>
       <c r="J31" s="104">
         <f t="shared" si="12"/>
-        <v>41500</v>
+        <v>20750</v>
       </c>
       <c r="K31" s="104">
         <f t="shared" si="12"/>
-        <v>45980</v>
+        <v>25080</v>
       </c>
       <c r="L31" s="104">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>43000</v>
       </c>
       <c r="M31" s="104">
         <f t="shared" si="12"/>
@@ -8286,23 +8252,23 @@
       </c>
       <c r="H32" s="108">
         <f t="shared" ref="H32:P32" si="13">H31-H29</f>
-        <v>13760</v>
+        <v>10320</v>
       </c>
       <c r="I32" s="108">
         <f t="shared" si="13"/>
-        <v>13360</v>
+        <v>11640</v>
       </c>
       <c r="J32" s="108">
         <f t="shared" si="13"/>
-        <v>17000</v>
+        <v>8450</v>
       </c>
       <c r="K32" s="108">
         <f t="shared" si="13"/>
-        <v>18980</v>
+        <v>10380</v>
       </c>
       <c r="L32" s="108">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>18400</v>
       </c>
       <c r="M32" s="108">
         <f t="shared" si="13"/>
@@ -8335,23 +8301,23 @@
       </c>
       <c r="H33" s="79">
         <f>SUM(J14:J15)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I33" s="79">
         <f t="shared" ref="I33:P33" si="14">SUM(K14:K15)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J33" s="79">
         <f t="shared" si="14"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K33" s="79">
         <f t="shared" si="14"/>
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="L33" s="79">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M33" s="79">
         <f t="shared" si="14"/>
@@ -8402,7 +8368,7 @@
       </c>
       <c r="J34" s="79">
         <f t="shared" si="15"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K34" s="79">
         <f t="shared" si="15"/>
@@ -8453,7 +8419,7 @@
       </c>
       <c r="J35" s="263">
         <f t="shared" si="16"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K35" s="263">
         <f t="shared" si="16"/>
@@ -8576,7 +8542,7 @@
       </c>
       <c r="J37" s="83">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" s="83">
         <f t="shared" si="18"/>
@@ -8670,7 +8636,7 @@
       </c>
       <c r="J38" s="130">
         <f t="shared" si="19"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="K38" s="130">
         <f t="shared" si="19"/>
@@ -8767,7 +8733,7 @@
       </c>
       <c r="J39" s="138">
         <f t="shared" si="28"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="K39" s="138">
         <f>K35*K27</f>
@@ -8862,7 +8828,7 @@
       </c>
       <c r="J40" s="108">
         <f t="shared" si="30"/>
-        <v>4900</v>
+        <v>0</v>
       </c>
       <c r="K40" s="108">
         <f t="shared" si="30"/>
@@ -8956,7 +8922,7 @@
       </c>
       <c r="J41" s="138">
         <f t="shared" si="31"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="K41" s="138">
         <f>K35*K30</f>
@@ -9050,7 +9016,7 @@
       </c>
       <c r="J42" s="141">
         <f t="shared" si="33"/>
-        <v>3400</v>
+        <v>0</v>
       </c>
       <c r="K42" s="141">
         <f t="shared" si="33"/>
@@ -9138,23 +9104,23 @@
       </c>
       <c r="H43" s="146">
         <f>H32-H42</f>
-        <v>13760</v>
+        <v>10320</v>
       </c>
       <c r="I43" s="146">
         <f t="shared" ref="I43:P43" si="34">I32-I42</f>
-        <v>13360</v>
+        <v>11640</v>
       </c>
       <c r="J43" s="146">
         <f t="shared" si="34"/>
-        <v>13600</v>
+        <v>8450</v>
       </c>
       <c r="K43" s="146">
         <f t="shared" si="34"/>
-        <v>18980</v>
+        <v>10380</v>
       </c>
       <c r="L43" s="146">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>18400</v>
       </c>
       <c r="M43" s="146">
         <f t="shared" si="34"/>
@@ -9231,11 +9197,11 @@
       </c>
       <c r="H44" s="150">
         <f t="shared" ref="H44:P44" si="35">H33/H23</f>
-        <v>0.375</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="I44" s="150">
         <f t="shared" si="35"/>
-        <v>0.25</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="J44" s="150">
         <f t="shared" si="35"/>
@@ -9243,11 +9209,11 @@
       </c>
       <c r="K44" s="150">
         <f t="shared" si="35"/>
-        <v>0.63636363636363635</v>
-      </c>
-      <c r="L44" s="150" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L44" s="150">
         <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M44" s="150">
         <f t="shared" si="35"/>
@@ -9332,15 +9298,15 @@
       </c>
       <c r="J45" s="150">
         <f t="shared" si="36"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K45" s="150">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="L45" s="150" t="e">
+      <c r="L45" s="150">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M45" s="150">
         <f t="shared" si="36"/>
@@ -9425,15 +9391,15 @@
       </c>
       <c r="J46" s="150">
         <f t="shared" si="37"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K46" s="150">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="L46" s="150" t="e">
+      <c r="L46" s="150">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M46" s="150">
         <f t="shared" si="37"/>
@@ -10091,7 +10057,7 @@
       </c>
       <c r="H58" s="245">
         <f>'DC2'!D13</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I58" s="245">
         <f>'DC2'!E13</f>
@@ -10107,15 +10073,15 @@
       </c>
       <c r="L58" s="245">
         <f>'DC2'!H13</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="M58" s="245">
         <f>'DC2'!I13</f>
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="N58" s="245">
         <f>'DC2'!J13</f>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O58" s="245">
         <f>'DC2'!K13</f>
@@ -10463,7 +10429,7 @@
       </c>
       <c r="H62" s="61">
         <f t="shared" ref="H62:O62" si="38">SUM(H58:H61)</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I62" s="61">
         <f t="shared" si="38"/>
@@ -10479,15 +10445,15 @@
       </c>
       <c r="L62" s="61">
         <f t="shared" si="38"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="M62" s="61">
         <f t="shared" si="38"/>
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="N62" s="61">
         <f t="shared" si="38"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O62" s="61">
         <f t="shared" si="38"/>
@@ -10628,39 +10594,39 @@
       </c>
       <c r="H64" s="68">
         <f t="shared" ref="H64:P64" si="39">G64+H63+H66-H62</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I64" s="68">
         <f t="shared" si="39"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J64" s="68">
         <f t="shared" si="39"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K64" s="68">
         <f t="shared" si="39"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L64" s="68">
         <f t="shared" si="39"/>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M64" s="68">
         <f t="shared" si="39"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="N64" s="68">
         <f t="shared" si="39"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="O64" s="68">
         <f t="shared" si="39"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P64" s="69">
         <f t="shared" si="39"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="R64" s="70" t="s">
         <v>45</v>
@@ -10727,7 +10693,7 @@
       </c>
       <c r="H65" s="68">
         <f t="shared" ref="H65:P65" si="40">IF(G64-H62+H63&lt;=$F$56, H62-H63-G64+$F$56,0)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I65" s="68">
         <f t="shared" si="40"/>
@@ -10735,31 +10701,31 @@
       </c>
       <c r="J65" s="68">
         <f t="shared" si="40"/>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="K65" s="68">
         <f t="shared" si="40"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L65" s="68">
         <f t="shared" si="40"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M65" s="68">
         <f t="shared" si="40"/>
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="N65" s="68">
         <f t="shared" si="40"/>
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="O65" s="68">
         <f t="shared" si="40"/>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="P65" s="69">
         <f t="shared" si="40"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R65" s="70" t="s">
         <v>48</v>
@@ -10823,7 +10789,7 @@
       </c>
       <c r="H66" s="68">
         <f t="shared" si="41"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I66" s="68">
         <f t="shared" si="41"/>
@@ -10835,7 +10801,7 @@
       </c>
       <c r="K66" s="68">
         <f t="shared" si="41"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L66" s="68">
         <f t="shared" si="41"/>
@@ -10843,19 +10809,19 @@
       </c>
       <c r="M66" s="68">
         <f t="shared" si="41"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N66" s="68">
         <f t="shared" si="41"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O66" s="68">
         <f t="shared" si="41"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="P66" s="69">
         <f t="shared" si="41"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="W66">
         <f t="shared" si="20"/>
@@ -10912,7 +10878,7 @@
       <c r="F67" s="74"/>
       <c r="G67" s="75">
         <f>H66</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H67" s="75">
         <f t="shared" ref="H67:P67" si="42">I66</f>
@@ -10924,7 +10890,7 @@
       </c>
       <c r="J67" s="75">
         <f t="shared" si="42"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K67" s="75">
         <f t="shared" si="42"/>
@@ -10932,19 +10898,19 @@
       </c>
       <c r="L67" s="75">
         <f t="shared" si="42"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="M67" s="75">
         <f t="shared" si="42"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N67" s="75">
         <f t="shared" si="42"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="O67" s="75">
         <f t="shared" si="42"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P67" s="76">
         <f t="shared" si="42"/>
@@ -11091,7 +11057,7 @@
       <c r="F69" s="153"/>
       <c r="G69" s="83">
         <f>QUOTIENT(G67+$F$50-1,$F$49)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H69" s="83">
         <f t="shared" ref="H69:P69" si="44">QUOTIENT(H67+$F$50-1,$F$49)</f>
@@ -11103,7 +11069,7 @@
       </c>
       <c r="J69" s="83">
         <f t="shared" si="44"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K69" s="83">
         <f t="shared" si="44"/>
@@ -11111,19 +11077,19 @@
       </c>
       <c r="L69" s="83">
         <f t="shared" si="44"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M69" s="83">
         <f t="shared" si="44"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N69" s="83">
         <f t="shared" si="44"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O69" s="83">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P69" s="84">
         <f t="shared" si="44"/>
@@ -11180,7 +11146,7 @@
       <c r="F70" s="86"/>
       <c r="G70" s="87">
         <f>IF($Q$70="Choosing Supplier 1", G69*$G$49+G68*$G$50,G69*$G$51+G68*$G$52)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H70" s="87">
         <f t="shared" ref="H70:P70" si="45">IF($Q$70="Choosing Supplier 1", H69*$G$49+H68*$G$50,H69*$G$51+H68*$G$52)</f>
@@ -11192,7 +11158,7 @@
       </c>
       <c r="J70" s="87">
         <f t="shared" si="45"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K70" s="87">
         <f t="shared" si="45"/>
@@ -11200,19 +11166,19 @@
       </c>
       <c r="L70" s="87">
         <f t="shared" si="45"/>
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="M70" s="87">
         <f t="shared" si="45"/>
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="N70" s="87">
         <f t="shared" si="45"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="O70" s="87">
         <f t="shared" si="45"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="P70" s="88">
         <f t="shared" si="45"/>
@@ -11368,7 +11334,7 @@
       <c r="F72" s="94"/>
       <c r="G72" s="95">
         <f t="shared" ref="G72:P72" si="46">G71*G67</f>
-        <v>8400</v>
+        <v>4200</v>
       </c>
       <c r="H72" s="95">
         <f t="shared" si="46"/>
@@ -11380,7 +11346,7 @@
       </c>
       <c r="J72" s="95">
         <f t="shared" si="46"/>
-        <v>12900</v>
+        <v>17200</v>
       </c>
       <c r="K72" s="95">
         <f t="shared" si="46"/>
@@ -11388,19 +11354,19 @@
       </c>
       <c r="L72" s="95">
         <f t="shared" si="46"/>
-        <v>21600</v>
+        <v>12960</v>
       </c>
       <c r="M72" s="95">
         <f t="shared" si="46"/>
-        <v>21400</v>
+        <v>12840</v>
       </c>
       <c r="N72" s="95">
         <f t="shared" si="46"/>
-        <v>8480</v>
+        <v>12720</v>
       </c>
       <c r="O72" s="95">
         <f t="shared" si="46"/>
-        <v>4200</v>
+        <v>0</v>
       </c>
       <c r="P72" s="134">
         <f t="shared" si="46"/>
@@ -11460,7 +11426,7 @@
       <c r="F73" s="99"/>
       <c r="G73" s="100">
         <f t="shared" ref="G73:P73" si="47">G70+G72</f>
-        <v>9400</v>
+        <v>4700</v>
       </c>
       <c r="H73" s="100">
         <f t="shared" si="47"/>
@@ -11472,7 +11438,7 @@
       </c>
       <c r="J73" s="100">
         <f t="shared" si="47"/>
-        <v>14400</v>
+        <v>19200</v>
       </c>
       <c r="K73" s="100">
         <f t="shared" si="47"/>
@@ -11480,19 +11446,19 @@
       </c>
       <c r="L73" s="100">
         <f t="shared" si="47"/>
-        <v>24100</v>
+        <v>14460</v>
       </c>
       <c r="M73" s="100">
         <f t="shared" si="47"/>
-        <v>23900</v>
+        <v>14340</v>
       </c>
       <c r="N73" s="100">
         <f t="shared" si="47"/>
-        <v>9480</v>
+        <v>14220</v>
       </c>
       <c r="O73" s="100">
         <f t="shared" si="47"/>
-        <v>4700</v>
+        <v>0</v>
       </c>
       <c r="P73" s="101">
         <f t="shared" si="47"/>
@@ -11641,7 +11607,7 @@
       <c r="F75" s="103"/>
       <c r="G75" s="104">
         <f>G74*G67</f>
-        <v>16440</v>
+        <v>8220</v>
       </c>
       <c r="H75" s="104">
         <f t="shared" ref="H75:P75" si="48">H74*H67</f>
@@ -11653,7 +11619,7 @@
       </c>
       <c r="J75" s="104">
         <f t="shared" si="48"/>
-        <v>24780</v>
+        <v>33040</v>
       </c>
       <c r="K75" s="104">
         <f t="shared" si="48"/>
@@ -11661,19 +11627,19 @@
       </c>
       <c r="L75" s="104">
         <f t="shared" si="48"/>
-        <v>42800</v>
+        <v>25680</v>
       </c>
       <c r="M75" s="104">
         <f t="shared" si="48"/>
-        <v>42600</v>
+        <v>25560</v>
       </c>
       <c r="N75" s="104">
         <f t="shared" si="48"/>
-        <v>16760</v>
+        <v>25140</v>
       </c>
       <c r="O75" s="104">
         <f t="shared" si="48"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="P75" s="105">
         <f t="shared" si="48"/>
@@ -11733,7 +11699,7 @@
       <c r="F76" s="107"/>
       <c r="G76" s="108">
         <f>G75-G73</f>
-        <v>7040</v>
+        <v>3520</v>
       </c>
       <c r="H76" s="108">
         <f t="shared" ref="H76:P76" si="49">H75-H73</f>
@@ -11745,7 +11711,7 @@
       </c>
       <c r="J76" s="108">
         <f t="shared" si="49"/>
-        <v>10380</v>
+        <v>13840</v>
       </c>
       <c r="K76" s="108">
         <f t="shared" si="49"/>
@@ -11753,19 +11719,19 @@
       </c>
       <c r="L76" s="108">
         <f t="shared" si="49"/>
-        <v>18700</v>
+        <v>11220</v>
       </c>
       <c r="M76" s="108">
         <f t="shared" si="49"/>
-        <v>18700</v>
+        <v>11220</v>
       </c>
       <c r="N76" s="108">
         <f t="shared" si="49"/>
-        <v>7280</v>
+        <v>10920</v>
       </c>
       <c r="O76" s="108">
         <f t="shared" si="49"/>
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="P76" s="109">
         <f t="shared" si="49"/>
@@ -11825,7 +11791,7 @@
       <c r="F77" s="215"/>
       <c r="G77" s="216">
         <f>SUM(H58:H59)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H77" s="216">
         <f t="shared" ref="H77:P77" si="50">SUM(I58:I59)</f>
@@ -11841,15 +11807,15 @@
       </c>
       <c r="K77" s="216">
         <f t="shared" si="50"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L77" s="216">
         <f t="shared" si="50"/>
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="M77" s="216">
         <f t="shared" si="50"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N77" s="216">
         <f t="shared" si="50"/>
@@ -11929,7 +11895,7 @@
       </c>
       <c r="J78" s="79">
         <f t="shared" si="51"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K78" s="79">
         <f t="shared" si="51"/>
@@ -11941,7 +11907,7 @@
       </c>
       <c r="M78" s="79">
         <f t="shared" si="51"/>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="N78" s="79">
         <f t="shared" si="51"/>
@@ -12019,7 +11985,7 @@
       </c>
       <c r="J79" s="263">
         <f t="shared" si="52"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K79" s="263">
         <f t="shared" si="52"/>
@@ -12031,7 +11997,7 @@
       </c>
       <c r="M79" s="263">
         <f t="shared" si="52"/>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="N79" s="263">
         <f t="shared" si="52"/>
@@ -12160,7 +12126,7 @@
       </c>
       <c r="J81" s="83">
         <f t="shared" si="54"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K81" s="83">
         <f t="shared" si="54"/>
@@ -12172,7 +12138,7 @@
       </c>
       <c r="M81" s="83">
         <f t="shared" si="54"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N81" s="83">
         <f t="shared" si="54"/>
@@ -12250,7 +12216,7 @@
       </c>
       <c r="J82" s="130">
         <f t="shared" si="55"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K82" s="130">
         <f t="shared" si="55"/>
@@ -12262,7 +12228,7 @@
       </c>
       <c r="M82" s="130">
         <f t="shared" si="55"/>
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="N82" s="130">
         <f t="shared" si="55"/>
@@ -12343,7 +12309,7 @@
       </c>
       <c r="J83" s="138">
         <f t="shared" si="56"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="K83" s="138">
         <f>K79*K71</f>
@@ -12355,7 +12321,7 @@
       </c>
       <c r="M83" s="138">
         <f t="shared" si="57"/>
-        <v>9630</v>
+        <v>3210</v>
       </c>
       <c r="N83" s="138">
         <f t="shared" si="57"/>
@@ -12434,7 +12400,7 @@
       </c>
       <c r="J84" s="108">
         <f t="shared" si="58"/>
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="K84" s="108">
         <f t="shared" si="58"/>
@@ -12446,7 +12412,7 @@
       </c>
       <c r="M84" s="108">
         <f t="shared" si="58"/>
-        <v>11130</v>
+        <v>3710</v>
       </c>
       <c r="N84" s="108">
         <f t="shared" si="58"/>
@@ -12482,7 +12448,7 @@
       </c>
       <c r="J85" s="138">
         <f t="shared" si="59"/>
-        <v>8260</v>
+        <v>0</v>
       </c>
       <c r="K85" s="138">
         <f>K79*K74</f>
@@ -12494,7 +12460,7 @@
       </c>
       <c r="M85" s="138">
         <f t="shared" si="60"/>
-        <v>19170</v>
+        <v>6390</v>
       </c>
       <c r="N85" s="138">
         <f t="shared" si="60"/>
@@ -12530,7 +12496,7 @@
       </c>
       <c r="J86" s="141">
         <f t="shared" si="61"/>
-        <v>3460</v>
+        <v>0</v>
       </c>
       <c r="K86" s="141">
         <f t="shared" si="61"/>
@@ -12542,7 +12508,7 @@
       </c>
       <c r="M86" s="141">
         <f t="shared" si="61"/>
-        <v>8040</v>
+        <v>2680</v>
       </c>
       <c r="N86" s="141">
         <f t="shared" si="61"/>
@@ -12568,7 +12534,7 @@
       <c r="F87" s="145"/>
       <c r="G87" s="146">
         <f>G76-G86</f>
-        <v>7040</v>
+        <v>3520</v>
       </c>
       <c r="H87" s="146">
         <f>H76-H86</f>
@@ -12580,7 +12546,7 @@
       </c>
       <c r="J87" s="146">
         <f t="shared" si="62"/>
-        <v>6920</v>
+        <v>13840</v>
       </c>
       <c r="K87" s="146">
         <f t="shared" si="62"/>
@@ -12588,19 +12554,19 @@
       </c>
       <c r="L87" s="146">
         <f t="shared" si="62"/>
-        <v>18700</v>
+        <v>11220</v>
       </c>
       <c r="M87" s="146">
         <f t="shared" si="62"/>
-        <v>10660</v>
+        <v>8540</v>
       </c>
       <c r="N87" s="146">
         <f t="shared" si="62"/>
-        <v>7280</v>
+        <v>10920</v>
       </c>
       <c r="O87" s="146">
         <f t="shared" si="62"/>
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="P87" s="147">
         <f t="shared" si="62"/>
@@ -12627,15 +12593,15 @@
       </c>
       <c r="J88" s="150">
         <f t="shared" si="63"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="K88" s="150">
         <f t="shared" si="63"/>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="L88" s="150">
         <f t="shared" si="63"/>
-        <v>0.6</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M88" s="150">
         <f t="shared" si="63"/>
@@ -12645,9 +12611,9 @@
         <f t="shared" si="63"/>
         <v>0</v>
       </c>
-      <c r="O88" s="150">
+      <c r="O88" s="150" t="e">
         <f t="shared" si="63"/>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P88" s="150" t="e">
         <f t="shared" si="63"/>
@@ -12674,7 +12640,7 @@
       </c>
       <c r="J89" s="150">
         <f t="shared" si="64"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K89" s="150">
         <f t="shared" si="64"/>
@@ -12686,15 +12652,15 @@
       </c>
       <c r="M89" s="150">
         <f t="shared" si="64"/>
-        <v>0.46569037656903767</v>
+        <v>0.25871687587168757</v>
       </c>
       <c r="N89" s="150">
         <f t="shared" si="64"/>
         <v>0</v>
       </c>
-      <c r="O89" s="150">
+      <c r="O89" s="150" t="e">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P89" s="150" t="e">
         <f t="shared" si="64"/>
@@ -12721,7 +12687,7 @@
       </c>
       <c r="J90" s="150">
         <f t="shared" si="65"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K90" s="150">
         <f t="shared" si="65"/>
@@ -12733,15 +12699,15 @@
       </c>
       <c r="M90" s="150">
         <f t="shared" si="65"/>
-        <v>0.42994652406417111</v>
+        <v>0.23885918003565063</v>
       </c>
       <c r="N90" s="150">
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
-      <c r="O90" s="150">
+      <c r="O90" s="150" t="e">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P90" s="150" t="e">
         <f t="shared" si="65"/>
@@ -12961,7 +12927,7 @@
       </c>
       <c r="L103" s="65">
         <f>'DC3'!H13</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M103" s="65">
         <f>'DC3'!I13</f>
@@ -13145,7 +13111,7 @@
       </c>
       <c r="L107" s="207">
         <f t="shared" si="66"/>
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="M107" s="207">
         <f t="shared" si="66"/>
@@ -13265,7 +13231,7 @@
       </c>
       <c r="L110" s="68">
         <f t="shared" si="68"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M110" s="68">
         <f t="shared" si="68"/>
@@ -13314,7 +13280,7 @@
       </c>
       <c r="L111" s="175">
         <f t="shared" si="69"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M111" s="175">
         <f t="shared" si="69"/>
@@ -13360,7 +13326,7 @@
       </c>
       <c r="L112" s="75">
         <f t="shared" si="70"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M112" s="75">
         <f t="shared" si="70"/>
@@ -13453,7 +13419,7 @@
       </c>
       <c r="L114" s="83">
         <f t="shared" si="72"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M114" s="83">
         <f t="shared" si="72"/>
@@ -13499,7 +13465,7 @@
       </c>
       <c r="L115" s="87">
         <f t="shared" si="73"/>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="M115" s="87">
         <f t="shared" si="73"/>
@@ -13601,7 +13567,7 @@
       </c>
       <c r="L117" s="95">
         <f t="shared" si="74"/>
-        <v>3240</v>
+        <v>12960</v>
       </c>
       <c r="M117" s="95">
         <f t="shared" si="74"/>
@@ -13650,7 +13616,7 @@
       </c>
       <c r="L118" s="100">
         <f t="shared" si="75"/>
-        <v>3440</v>
+        <v>13560</v>
       </c>
       <c r="M118" s="100">
         <f t="shared" si="75"/>
@@ -13745,7 +13711,7 @@
       </c>
       <c r="L120" s="104">
         <f t="shared" si="76"/>
-        <v>6450</v>
+        <v>25800</v>
       </c>
       <c r="M120" s="104">
         <f t="shared" si="76"/>
@@ -13794,7 +13760,7 @@
       </c>
       <c r="L121" s="108">
         <f t="shared" si="77"/>
-        <v>3010</v>
+        <v>12240</v>
       </c>
       <c r="M121" s="108">
         <f t="shared" si="77"/>
@@ -13857,7 +13823,7 @@
       </c>
       <c r="L122" s="216">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M122" s="216">
         <f t="shared" si="78"/>
@@ -13912,7 +13878,7 @@
       </c>
       <c r="J123" s="79">
         <f t="shared" si="79"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K123" s="79">
         <f t="shared" si="79"/>
@@ -13924,7 +13890,7 @@
       </c>
       <c r="M123" s="79">
         <f t="shared" si="79"/>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="N123" s="79">
         <f t="shared" si="79"/>
@@ -13973,7 +13939,7 @@
       </c>
       <c r="J124" s="263">
         <f t="shared" si="80"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K124" s="263">
         <f t="shared" si="80"/>
@@ -13985,7 +13951,7 @@
       </c>
       <c r="M124" s="263">
         <f t="shared" si="80"/>
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N124" s="263">
         <f t="shared" si="80"/>
@@ -14095,7 +14061,7 @@
       </c>
       <c r="J126" s="83">
         <f t="shared" si="82"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K126" s="83">
         <f t="shared" si="82"/>
@@ -14107,7 +14073,7 @@
       </c>
       <c r="M126" s="83">
         <f t="shared" si="82"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N126" s="83">
         <f t="shared" si="82"/>
@@ -14156,7 +14122,7 @@
       </c>
       <c r="J127" s="130">
         <f t="shared" si="83"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="K127" s="130">
         <f t="shared" si="83"/>
@@ -14168,7 +14134,7 @@
       </c>
       <c r="M127" s="130">
         <f t="shared" si="83"/>
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="N127" s="130">
         <f t="shared" si="83"/>
@@ -14220,7 +14186,7 @@
       </c>
       <c r="J128" s="138">
         <f t="shared" si="84"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="K128" s="138">
         <f>K124*K116</f>
@@ -14232,7 +14198,7 @@
       </c>
       <c r="M128" s="138">
         <f t="shared" si="85"/>
-        <v>11770</v>
+        <v>5350</v>
       </c>
       <c r="N128" s="138">
         <f t="shared" si="85"/>
@@ -14282,7 +14248,7 @@
       </c>
       <c r="J129" s="108">
         <f t="shared" si="86"/>
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="K129" s="108">
         <f t="shared" si="86"/>
@@ -14294,7 +14260,7 @@
       </c>
       <c r="M129" s="108">
         <f t="shared" si="86"/>
-        <v>12370</v>
+        <v>5550</v>
       </c>
       <c r="N129" s="108">
         <f t="shared" si="86"/>
@@ -14343,7 +14309,7 @@
       </c>
       <c r="J130" s="138">
         <f t="shared" si="87"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="K130" s="138">
         <f>K124*K119</f>
@@ -14355,7 +14321,7 @@
       </c>
       <c r="M130" s="138">
         <f t="shared" si="88"/>
-        <v>23265</v>
+        <v>10575</v>
       </c>
       <c r="N130" s="138">
         <f t="shared" si="88"/>
@@ -14390,7 +14356,7 @@
       </c>
       <c r="J131" s="141">
         <f t="shared" si="89"/>
-        <v>3800</v>
+        <v>0</v>
       </c>
       <c r="K131" s="141">
         <f t="shared" si="89"/>
@@ -14402,7 +14368,7 @@
       </c>
       <c r="M131" s="141">
         <f t="shared" si="89"/>
-        <v>10895</v>
+        <v>5025</v>
       </c>
       <c r="N131" s="141">
         <f t="shared" si="89"/>
@@ -14439,7 +14405,7 @@
       </c>
       <c r="J132" s="146">
         <f t="shared" si="90"/>
-        <v>7600</v>
+        <v>11400</v>
       </c>
       <c r="K132" s="146">
         <f t="shared" si="90"/>
@@ -14447,11 +14413,11 @@
       </c>
       <c r="L132" s="146">
         <f t="shared" si="90"/>
-        <v>3010</v>
+        <v>12240</v>
       </c>
       <c r="M132" s="146">
         <f t="shared" si="90"/>
-        <v>15920</v>
+        <v>21790</v>
       </c>
       <c r="N132" s="146">
         <f t="shared" si="90"/>
@@ -14494,7 +14460,7 @@
       </c>
       <c r="L133" s="150">
         <f t="shared" si="91"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="M133" s="150">
         <f t="shared" si="91"/>
@@ -14533,7 +14499,7 @@
       </c>
       <c r="J134" s="150">
         <f t="shared" si="92"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K134" s="150">
         <f t="shared" si="92"/>
@@ -14545,7 +14511,7 @@
       </c>
       <c r="M134" s="150">
         <f t="shared" si="92"/>
-        <v>0.40838560581049854</v>
+        <v>0.18322878837900297</v>
       </c>
       <c r="N134" s="150">
         <f t="shared" si="92"/>
@@ -14580,7 +14546,7 @@
       </c>
       <c r="J135" s="150">
         <f t="shared" si="93"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K135" s="150">
         <f t="shared" si="93"/>
@@ -14592,7 +14558,7 @@
       </c>
       <c r="M135" s="150">
         <f t="shared" si="93"/>
-        <v>0.40630244266268878</v>
+        <v>0.18739511467462242</v>
       </c>
       <c r="N135" s="150">
         <f t="shared" si="93"/>
@@ -14664,7 +14630,7 @@
       </c>
       <c r="F141" s="6">
         <f>Supplier1!C7</f>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G141" t="s">
         <v>35</v>
@@ -14697,7 +14663,7 @@
       </c>
       <c r="F143" s="7">
         <f>Supplier1!C4</f>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="O143" s="301"/>
       <c r="P143" s="301"/>
@@ -14762,23 +14728,23 @@
       </c>
       <c r="H146" s="282">
         <f t="shared" ref="H146:P146" si="94">IF($Q$26 = "Choosing Supplier 1", IF($F$144="Yes", H23,0),0)</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I146" s="282">
         <f t="shared" si="94"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="J146" s="282">
         <f t="shared" si="94"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K146" s="282">
         <f t="shared" si="94"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="L146" s="282">
         <f t="shared" si="94"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M146" s="282">
         <f t="shared" si="94"/>
@@ -14804,7 +14770,7 @@
       <c r="F147" s="271"/>
       <c r="G147" s="272">
         <f>IF($Q$70 = "Choosing Supplier 1", IF($F$144="Yes", G67,0),0)</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H147" s="272">
         <f t="shared" ref="H147:P147" si="95">IF($Q$70 = "Choosing Supplier 1", IF($F$144="Yes", H67,0),0)</f>
@@ -14816,7 +14782,7 @@
       </c>
       <c r="J147" s="272">
         <f t="shared" si="95"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K147" s="272">
         <f t="shared" si="95"/>
@@ -14824,19 +14790,19 @@
       </c>
       <c r="L147" s="272">
         <f t="shared" si="95"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="M147" s="272">
         <f t="shared" si="95"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N147" s="272">
         <f t="shared" si="95"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="O147" s="272">
         <f t="shared" si="95"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P147" s="273">
         <f t="shared" si="95"/>
@@ -14870,7 +14836,7 @@
       </c>
       <c r="L148" s="275">
         <f t="shared" si="96"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M148" s="275">
         <f t="shared" si="96"/>
@@ -14896,39 +14862,39 @@
       <c r="F149" s="186"/>
       <c r="G149" s="287">
         <f>SUM(G146:G148)</f>
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="H149" s="287">
         <f t="shared" ref="H149:P149" si="97">SUM(H146:H148)</f>
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="I149" s="287">
         <f t="shared" si="97"/>
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J149" s="287">
         <f t="shared" si="97"/>
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="K149" s="287">
         <f t="shared" si="97"/>
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="L149" s="287">
         <f t="shared" si="97"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="M149" s="287">
         <f t="shared" si="97"/>
-        <v>275</v>
+        <v>235</v>
       </c>
       <c r="N149" s="287">
         <f t="shared" si="97"/>
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O149" s="287">
         <f t="shared" si="97"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="P149" s="288">
         <f t="shared" si="97"/>
@@ -14961,7 +14927,7 @@
       </c>
       <c r="G151" s="68">
         <f t="shared" ref="G151:P151" si="98">F151+G153-G149</f>
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="H151" s="68">
         <f t="shared" si="98"/>
@@ -14969,35 +14935,35 @@
       </c>
       <c r="I151" s="68">
         <f t="shared" si="98"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J151" s="68">
         <f t="shared" si="98"/>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K151" s="68">
         <f t="shared" si="98"/>
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="L151" s="68">
         <f t="shared" si="98"/>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="M151" s="68">
         <f t="shared" si="98"/>
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="N151" s="68">
         <f t="shared" si="98"/>
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="O151" s="68">
         <f t="shared" si="98"/>
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="P151" s="69">
         <f t="shared" si="98"/>
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="152" spans="4:17" x14ac:dyDescent="0.3">
@@ -15007,7 +14973,7 @@
       <c r="F152" s="71"/>
       <c r="G152" s="68">
         <f t="shared" ref="G152:P152" si="99">IF(F151-G149&lt;=$F$142, G149-F151+$F$142,0)</f>
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="H152" s="68">
         <f t="shared" si="99"/>
@@ -15015,35 +14981,35 @@
       </c>
       <c r="I152" s="68">
         <f t="shared" si="99"/>
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="J152" s="68">
         <f t="shared" si="99"/>
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="K152" s="68">
         <f t="shared" si="99"/>
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="L152" s="68">
         <f t="shared" si="99"/>
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="M152" s="68">
         <f t="shared" si="99"/>
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="N152" s="68">
         <f t="shared" si="99"/>
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="O152" s="68">
         <f t="shared" si="99"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P152" s="69">
         <f t="shared" si="99"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="153" spans="4:17" x14ac:dyDescent="0.3">
@@ -15053,7 +15019,7 @@
       <c r="F153" s="71"/>
       <c r="G153" s="68">
         <f xml:space="preserve"> CEILING(G152/$F$141,1)*$F$141</f>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="H153" s="68">
         <f t="shared" ref="H153:P153" si="100" xml:space="preserve"> CEILING(H152/$F$141,1)*$F$141</f>
@@ -15061,35 +15027,35 @@
       </c>
       <c r="I153" s="68">
         <f t="shared" si="100"/>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="J153" s="68">
         <f t="shared" si="100"/>
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="K153" s="68">
         <f t="shared" si="100"/>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="L153" s="68">
         <f t="shared" si="100"/>
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="M153" s="68">
         <f t="shared" si="100"/>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="N153" s="68">
         <f t="shared" si="100"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="O153" s="68">
         <f t="shared" si="100"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="P153" s="69">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="154" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15103,35 +15069,35 @@
       </c>
       <c r="H154" s="195">
         <f>I153</f>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="I154" s="195">
         <f t="shared" ref="I154:P154" si="101">J153</f>
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="J154" s="195">
         <f t="shared" si="101"/>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="K154" s="195">
         <f t="shared" si="101"/>
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="L154" s="195">
         <f t="shared" si="101"/>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="M154" s="195">
         <f t="shared" si="101"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="N154" s="195">
         <f t="shared" si="101"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="O154" s="195">
         <f t="shared" si="101"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P154" s="196">
         <f t="shared" si="101"/>
@@ -15158,7 +15124,7 @@
       </c>
       <c r="J155" s="199">
         <f t="shared" si="102"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K155" s="199">
         <f t="shared" si="102"/>
@@ -15170,7 +15136,7 @@
       </c>
       <c r="M155" s="199">
         <f t="shared" si="102"/>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="N155" s="199">
         <f t="shared" si="102"/>
@@ -15205,7 +15171,7 @@
       </c>
       <c r="J156" s="199">
         <f t="shared" si="102"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K156" s="199">
         <f t="shared" si="102"/>
@@ -15217,7 +15183,7 @@
       </c>
       <c r="M156" s="199">
         <f t="shared" si="102"/>
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="N156" s="199">
         <f t="shared" si="102"/>
@@ -15305,7 +15271,7 @@
       </c>
       <c r="F164" s="7">
         <f>Supplier2!C4</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="O164" s="301"/>
       <c r="P164" s="301"/>
@@ -15948,8 +15914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B409AB02-E9CA-40CB-B386-70D450CE0A6B}">
   <dimension ref="A2:AK192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q175" sqref="Q175"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J165" sqref="J165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16179,23 +16145,23 @@
       </c>
       <c r="J14" s="245">
         <f>'DC1'!F13</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="K14" s="248">
         <f>'DC1'!G13</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L14" s="245">
         <f>'DC1'!H13</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M14" s="245">
         <f>'DC1'!I13</f>
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="N14" s="245">
         <f>'DC1'!J13</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O14" s="245">
         <f>'DC1'!K13</f>
@@ -16372,23 +16338,23 @@
       </c>
       <c r="J18" s="61">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="K18" s="61">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L18" s="61">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M18" s="61">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="N18" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O18" s="61">
         <f t="shared" si="0"/>
@@ -16446,7 +16412,7 @@
       </c>
       <c r="J20" s="68">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K20" s="68">
         <f t="shared" si="1"/>
@@ -16498,23 +16464,23 @@
       </c>
       <c r="J21" s="68">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="K21" s="68">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L21" s="68">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M21" s="68">
         <f t="shared" si="2"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="N21" s="68">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O21" s="68">
         <f t="shared" si="2"/>
@@ -16547,23 +16513,23 @@
       </c>
       <c r="J22" s="68">
         <f t="shared" ref="J22" si="4" xml:space="preserve"> CEILING(J21/$F$11,1)*$F$11</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="K22" s="68">
         <f t="shared" ref="K22:L22" si="5" xml:space="preserve"> CEILING(K21/$F$11,1)*$F$11</f>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L22" s="68">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M22" s="68">
         <f t="shared" ref="M22" si="6" xml:space="preserve"> CEILING(M21/$F$11,1)*$F$11</f>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="N22" s="68">
         <f t="shared" ref="N22:O22" si="7" xml:space="preserve"> CEILING(N21/$F$11,1)*$F$11</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O22" s="68">
         <f t="shared" si="7"/>
@@ -16585,23 +16551,23 @@
       </c>
       <c r="H23" s="75">
         <f t="shared" ref="H23:P23" si="9">IF($Q$26 = "Choosing Supplier 1", J22, I22)</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I23" s="75">
         <f t="shared" si="9"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="J23" s="75">
         <f t="shared" si="9"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K23" s="75">
         <f t="shared" si="9"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="L23" s="75">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M23" s="75">
         <f t="shared" si="9"/>
@@ -16635,15 +16601,15 @@
       </c>
       <c r="I24" s="79">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="79">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="79">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="79">
         <f t="shared" si="10"/>
@@ -16678,23 +16644,23 @@
       </c>
       <c r="H25" s="83">
         <f t="shared" ref="H25:P25" si="11">QUOTIENT(H23+$F$6-1,$F$5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I25" s="83">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J25" s="83">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K25" s="83">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L25" s="83">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M25" s="83">
         <f t="shared" si="11"/>
@@ -16724,23 +16690,23 @@
       </c>
       <c r="H26" s="87">
         <f t="shared" ref="H26:P26" si="12">IF($Q$26="Choosing Supplier 1", H25*$G$5+H24*$G$6,H25*$G$7+H24*$G$8)</f>
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="I26" s="87">
         <f t="shared" si="12"/>
-        <v>2400</v>
+        <v>2150</v>
       </c>
       <c r="J26" s="87">
         <f t="shared" si="12"/>
-        <v>3000</v>
+        <v>1550</v>
       </c>
       <c r="K26" s="87">
         <f t="shared" si="12"/>
-        <v>3350</v>
+        <v>1800</v>
       </c>
       <c r="L26" s="87">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="M26" s="87">
         <f t="shared" si="12"/>
@@ -16826,23 +16792,23 @@
       </c>
       <c r="H28" s="96">
         <f>H27*H23</f>
-        <v>16880</v>
+        <v>12660</v>
       </c>
       <c r="I28" s="96">
         <f t="shared" si="13"/>
-        <v>17040</v>
+        <v>14910</v>
       </c>
       <c r="J28" s="96">
         <f t="shared" si="13"/>
-        <v>21500</v>
+        <v>10750</v>
       </c>
       <c r="K28" s="96">
         <f t="shared" si="13"/>
-        <v>23650</v>
+        <v>12900</v>
       </c>
       <c r="L28" s="96">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>21600</v>
       </c>
       <c r="M28" s="96">
         <f t="shared" si="13"/>
@@ -16878,23 +16844,23 @@
       </c>
       <c r="H29" s="100">
         <f t="shared" si="14"/>
-        <v>19280</v>
+        <v>14460</v>
       </c>
       <c r="I29" s="100">
         <f t="shared" si="14"/>
-        <v>19440</v>
+        <v>17060</v>
       </c>
       <c r="J29" s="100">
         <f t="shared" si="14"/>
-        <v>24500</v>
+        <v>12300</v>
       </c>
       <c r="K29" s="100">
         <f t="shared" si="14"/>
-        <v>27000</v>
+        <v>14700</v>
       </c>
       <c r="L29" s="100">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>24600</v>
       </c>
       <c r="M29" s="100">
         <f t="shared" si="14"/>
@@ -16976,23 +16942,23 @@
       </c>
       <c r="H31" s="104">
         <f t="shared" ref="H31:P31" si="15">H30*H23</f>
-        <v>33040</v>
+        <v>24780</v>
       </c>
       <c r="I31" s="104">
         <f t="shared" si="15"/>
-        <v>32800</v>
+        <v>28700</v>
       </c>
       <c r="J31" s="104">
         <f t="shared" si="15"/>
-        <v>41500</v>
+        <v>20750</v>
       </c>
       <c r="K31" s="104">
         <f t="shared" si="15"/>
-        <v>45980</v>
+        <v>25080</v>
       </c>
       <c r="L31" s="104">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>43000</v>
       </c>
       <c r="M31" s="104">
         <f t="shared" si="15"/>
@@ -17025,23 +16991,23 @@
       </c>
       <c r="H32" s="108">
         <f t="shared" ref="H32:P32" si="16">H31-H29</f>
-        <v>13760</v>
+        <v>10320</v>
       </c>
       <c r="I32" s="108">
         <f t="shared" si="16"/>
-        <v>13360</v>
+        <v>11640</v>
       </c>
       <c r="J32" s="108">
         <f t="shared" si="16"/>
-        <v>17000</v>
+        <v>8450</v>
       </c>
       <c r="K32" s="108">
         <f t="shared" si="16"/>
-        <v>18980</v>
+        <v>10380</v>
       </c>
       <c r="L32" s="108">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>18400</v>
       </c>
       <c r="M32" s="108">
         <f t="shared" si="16"/>
@@ -17074,23 +17040,23 @@
       </c>
       <c r="H33" s="216">
         <f t="shared" si="17"/>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I33" s="216">
         <f>IF($Q$26 = "Choosing Supplier 1", SUM(K14:K15),SUM(J14:J15))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J33" s="216">
         <f t="shared" ref="J33:P33" si="18">IF($Q$26 = "Choosing Supplier 1", SUM(L14:L15),SUM(K14:K15))</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K33" s="216">
         <f t="shared" si="18"/>
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="L33" s="216">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M33" s="216">
         <f t="shared" si="18"/>
@@ -17141,7 +17107,7 @@
       </c>
       <c r="J34" s="79">
         <f t="shared" si="19"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K34" s="79">
         <f t="shared" si="19"/>
@@ -17192,7 +17158,7 @@
       </c>
       <c r="J35" s="299">
         <f t="shared" si="20"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K35" s="299">
         <f t="shared" si="20"/>
@@ -17243,7 +17209,7 @@
       </c>
       <c r="J36" s="263">
         <f t="shared" si="21"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K36" s="263">
         <f t="shared" si="21"/>
@@ -17374,7 +17340,7 @@
       </c>
       <c r="J38" s="83">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" s="83">
         <f>IF($Q$26="Choosing Supplier 1", QUOTIENT(K36+$F$6-1,$F$5),QUOTIENT(K36+$F$8-1,$F$7))</f>
@@ -17470,7 +17436,7 @@
       </c>
       <c r="J39" s="130">
         <f t="shared" si="26"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="K39" s="130">
         <f>IF($Q$26="Choosing Supplier 1", K38*$G$5+K37*$G$6, K38*$G$7+K37*$G$8)</f>
@@ -17569,7 +17535,7 @@
       </c>
       <c r="J40" s="138">
         <f t="shared" si="36"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="K40" s="138">
         <f>K36*K27</f>
@@ -17666,7 +17632,7 @@
       </c>
       <c r="J41" s="108">
         <f t="shared" si="38"/>
-        <v>4900</v>
+        <v>0</v>
       </c>
       <c r="K41" s="108">
         <f t="shared" si="38"/>
@@ -17762,7 +17728,7 @@
       </c>
       <c r="J42" s="138">
         <f t="shared" si="39"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="K42" s="138">
         <f>K36*K30</f>
@@ -17858,7 +17824,7 @@
       </c>
       <c r="J43" s="141">
         <f t="shared" si="41"/>
-        <v>3400</v>
+        <v>0</v>
       </c>
       <c r="K43" s="141">
         <f t="shared" si="41"/>
@@ -17949,23 +17915,23 @@
       </c>
       <c r="H44" s="146">
         <f>H32-H43</f>
-        <v>13760</v>
+        <v>10320</v>
       </c>
       <c r="I44" s="146">
         <f t="shared" ref="I44:P44" si="42">I32-I43</f>
-        <v>13360</v>
+        <v>11640</v>
       </c>
       <c r="J44" s="146">
         <f t="shared" si="42"/>
-        <v>13600</v>
+        <v>8450</v>
       </c>
       <c r="K44" s="146">
         <f t="shared" si="42"/>
-        <v>18980</v>
+        <v>10380</v>
       </c>
       <c r="L44" s="146">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>18400</v>
       </c>
       <c r="M44" s="146">
         <f t="shared" si="42"/>
@@ -18045,11 +18011,11 @@
       </c>
       <c r="H45" s="150">
         <f t="shared" ref="H45:P45" si="43">H33/H23</f>
-        <v>0.375</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="I45" s="150">
         <f t="shared" si="43"/>
-        <v>0.25</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="J45" s="150">
         <f t="shared" si="43"/>
@@ -18057,11 +18023,11 @@
       </c>
       <c r="K45" s="150">
         <f t="shared" si="43"/>
-        <v>0.63636363636363635</v>
-      </c>
-      <c r="L45" s="150" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L45" s="150">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M45" s="150">
         <f t="shared" si="43"/>
@@ -18146,15 +18112,15 @@
       </c>
       <c r="J46" s="150">
         <f t="shared" si="44"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K46" s="150">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="L46" s="150" t="e">
+      <c r="L46" s="150">
         <f t="shared" si="44"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M46" s="150">
         <f t="shared" si="44"/>
@@ -18239,15 +18205,15 @@
       </c>
       <c r="J47" s="150">
         <f t="shared" si="45"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K47" s="150">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="L47" s="150" t="e">
+      <c r="L47" s="150">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M47" s="150">
         <f t="shared" si="45"/>
@@ -18889,7 +18855,7 @@
       </c>
       <c r="H59" s="245">
         <f>'DC2'!D13</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I59" s="245">
         <f>'DC2'!E13</f>
@@ -18905,15 +18871,15 @@
       </c>
       <c r="L59" s="245">
         <f>'DC2'!H13</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="M59" s="245">
         <f>'DC2'!I13</f>
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="N59" s="245">
         <f>'DC2'!J13</f>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O59" s="245">
         <f>'DC2'!K13</f>
@@ -19261,7 +19227,7 @@
       </c>
       <c r="H63" s="61">
         <f t="shared" ref="H63:O63" si="46">SUM(H59:H62)</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I63" s="61">
         <f t="shared" si="46"/>
@@ -19277,15 +19243,15 @@
       </c>
       <c r="L63" s="61">
         <f t="shared" si="46"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="M63" s="61">
         <f t="shared" si="46"/>
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="N63" s="61">
         <f t="shared" si="46"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O63" s="61">
         <f t="shared" si="46"/>
@@ -19426,39 +19392,39 @@
       </c>
       <c r="H65" s="68">
         <f t="shared" ref="H65:P65" si="47">G65+H64+H67-H63</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I65" s="68">
         <f t="shared" si="47"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J65" s="68">
         <f t="shared" si="47"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K65" s="68">
         <f t="shared" si="47"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L65" s="68">
         <f t="shared" si="47"/>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M65" s="68">
         <f t="shared" si="47"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="N65" s="68">
         <f t="shared" si="47"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="O65" s="68">
         <f t="shared" si="47"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P65" s="69">
         <f t="shared" si="47"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="R65" s="70" t="s">
         <v>45</v>
@@ -19525,7 +19491,7 @@
       </c>
       <c r="H66" s="68">
         <f t="shared" ref="H66:P66" si="48">IF(G65-H63+H64&lt;=$F$57, H63-H64-G65+$F$57,0)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I66" s="68">
         <f t="shared" si="48"/>
@@ -19533,31 +19499,31 @@
       </c>
       <c r="J66" s="68">
         <f t="shared" si="48"/>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="K66" s="68">
         <f t="shared" si="48"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L66" s="68">
         <f t="shared" si="48"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M66" s="68">
         <f t="shared" si="48"/>
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="N66" s="68">
         <f t="shared" si="48"/>
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="O66" s="68">
         <f t="shared" si="48"/>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="P66" s="69">
         <f t="shared" si="48"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R66" s="70" t="s">
         <v>48</v>
@@ -19621,7 +19587,7 @@
       </c>
       <c r="H67" s="68">
         <f t="shared" si="49"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I67" s="68">
         <f t="shared" si="49"/>
@@ -19633,7 +19599,7 @@
       </c>
       <c r="K67" s="68">
         <f t="shared" si="49"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L67" s="68">
         <f t="shared" si="49"/>
@@ -19641,19 +19607,19 @@
       </c>
       <c r="M67" s="68">
         <f t="shared" si="49"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N67" s="68">
         <f t="shared" si="49"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O67" s="68">
         <f t="shared" si="49"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="P67" s="69">
         <f t="shared" si="49"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="W67">
         <f t="shared" si="28"/>
@@ -19710,7 +19676,7 @@
       <c r="F68" s="74"/>
       <c r="G68" s="75">
         <f>IF($Q$71 = "Choosing Supplier 1", H67, H67)</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H68" s="75">
         <f t="shared" ref="H68:P68" si="50">IF($Q$71 = "Choosing Supplier 1", I67, I67)</f>
@@ -19722,7 +19688,7 @@
       </c>
       <c r="J68" s="75">
         <f t="shared" si="50"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K68" s="75">
         <f t="shared" si="50"/>
@@ -19730,19 +19696,19 @@
       </c>
       <c r="L68" s="75">
         <f t="shared" si="50"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="M68" s="75">
         <f t="shared" si="50"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N68" s="75">
         <f t="shared" si="50"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="O68" s="75">
         <f t="shared" si="50"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P68" s="76">
         <f t="shared" si="50"/>
@@ -19889,7 +19855,7 @@
       <c r="F70" s="153"/>
       <c r="G70" s="83">
         <f>QUOTIENT(G68+$F$51-1,$F$50)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H70" s="83">
         <f t="shared" ref="H70:P70" si="52">QUOTIENT(H68+$F$51-1,$F$50)</f>
@@ -19901,7 +19867,7 @@
       </c>
       <c r="J70" s="83">
         <f t="shared" si="52"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K70" s="83">
         <f t="shared" si="52"/>
@@ -19909,19 +19875,19 @@
       </c>
       <c r="L70" s="83">
         <f t="shared" si="52"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M70" s="83">
         <f t="shared" si="52"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N70" s="83">
         <f t="shared" si="52"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O70" s="83">
         <f t="shared" si="52"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P70" s="84">
         <f t="shared" si="52"/>
@@ -19978,7 +19944,7 @@
       <c r="F71" s="86"/>
       <c r="G71" s="87">
         <f>IF($Q$71="Choosing Supplier 1", G70*$G$50+G69*$G$51,G70*$G$52+G69*$G$53)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H71" s="87">
         <f t="shared" ref="H71:P71" si="53">IF($Q$71="Choosing Supplier 1", H70*$G$50+H69*$G$51,H70*$G$52+H69*$G$53)</f>
@@ -19990,7 +19956,7 @@
       </c>
       <c r="J71" s="87">
         <f t="shared" si="53"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K71" s="87">
         <f t="shared" si="53"/>
@@ -19998,19 +19964,19 @@
       </c>
       <c r="L71" s="87">
         <f t="shared" si="53"/>
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="M71" s="87">
         <f t="shared" si="53"/>
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="N71" s="87">
         <f t="shared" si="53"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="O71" s="87">
         <f t="shared" si="53"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="P71" s="88">
         <f t="shared" si="53"/>
@@ -20166,7 +20132,7 @@
       <c r="F73" s="94"/>
       <c r="G73" s="95">
         <f t="shared" ref="G73:P73" si="54">G72*G68</f>
-        <v>8400</v>
+        <v>4200</v>
       </c>
       <c r="H73" s="95">
         <f t="shared" si="54"/>
@@ -20178,7 +20144,7 @@
       </c>
       <c r="J73" s="95">
         <f t="shared" si="54"/>
-        <v>12900</v>
+        <v>17200</v>
       </c>
       <c r="K73" s="95">
         <f t="shared" si="54"/>
@@ -20186,19 +20152,19 @@
       </c>
       <c r="L73" s="95">
         <f t="shared" si="54"/>
-        <v>21600</v>
+        <v>12960</v>
       </c>
       <c r="M73" s="95">
         <f t="shared" si="54"/>
-        <v>21400</v>
+        <v>12840</v>
       </c>
       <c r="N73" s="95">
         <f t="shared" si="54"/>
-        <v>8480</v>
+        <v>12720</v>
       </c>
       <c r="O73" s="95">
         <f t="shared" si="54"/>
-        <v>4200</v>
+        <v>0</v>
       </c>
       <c r="P73" s="134">
         <f t="shared" si="54"/>
@@ -20258,7 +20224,7 @@
       <c r="F74" s="99"/>
       <c r="G74" s="100">
         <f t="shared" ref="G74:P74" si="55">G71+G73</f>
-        <v>9400</v>
+        <v>4700</v>
       </c>
       <c r="H74" s="100">
         <f t="shared" si="55"/>
@@ -20270,7 +20236,7 @@
       </c>
       <c r="J74" s="100">
         <f t="shared" si="55"/>
-        <v>14400</v>
+        <v>19200</v>
       </c>
       <c r="K74" s="100">
         <f t="shared" si="55"/>
@@ -20278,19 +20244,19 @@
       </c>
       <c r="L74" s="100">
         <f t="shared" si="55"/>
-        <v>24100</v>
+        <v>14460</v>
       </c>
       <c r="M74" s="100">
         <f t="shared" si="55"/>
-        <v>23900</v>
+        <v>14340</v>
       </c>
       <c r="N74" s="100">
         <f t="shared" si="55"/>
-        <v>9480</v>
+        <v>14220</v>
       </c>
       <c r="O74" s="100">
         <f t="shared" si="55"/>
-        <v>4700</v>
+        <v>0</v>
       </c>
       <c r="P74" s="101">
         <f t="shared" si="55"/>
@@ -20439,7 +20405,7 @@
       <c r="F76" s="103"/>
       <c r="G76" s="104">
         <f>G75*G68</f>
-        <v>16440</v>
+        <v>8220</v>
       </c>
       <c r="H76" s="104">
         <f t="shared" ref="H76:P76" si="56">H75*H68</f>
@@ -20451,7 +20417,7 @@
       </c>
       <c r="J76" s="104">
         <f t="shared" si="56"/>
-        <v>24780</v>
+        <v>33040</v>
       </c>
       <c r="K76" s="104">
         <f t="shared" si="56"/>
@@ -20459,19 +20425,19 @@
       </c>
       <c r="L76" s="104">
         <f t="shared" si="56"/>
-        <v>42800</v>
+        <v>25680</v>
       </c>
       <c r="M76" s="104">
         <f t="shared" si="56"/>
-        <v>42600</v>
+        <v>25560</v>
       </c>
       <c r="N76" s="104">
         <f t="shared" si="56"/>
-        <v>16760</v>
+        <v>25140</v>
       </c>
       <c r="O76" s="104">
         <f t="shared" si="56"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="P76" s="105">
         <f t="shared" si="56"/>
@@ -20531,7 +20497,7 @@
       <c r="F77" s="107"/>
       <c r="G77" s="108">
         <f>G76-G74</f>
-        <v>7040</v>
+        <v>3520</v>
       </c>
       <c r="H77" s="108">
         <f t="shared" ref="H77:P77" si="57">H76-H74</f>
@@ -20543,7 +20509,7 @@
       </c>
       <c r="J77" s="108">
         <f t="shared" si="57"/>
-        <v>10380</v>
+        <v>13840</v>
       </c>
       <c r="K77" s="108">
         <f t="shared" si="57"/>
@@ -20551,19 +20517,19 @@
       </c>
       <c r="L77" s="108">
         <f t="shared" si="57"/>
-        <v>18700</v>
+        <v>11220</v>
       </c>
       <c r="M77" s="108">
         <f t="shared" si="57"/>
-        <v>18700</v>
+        <v>11220</v>
       </c>
       <c r="N77" s="108">
         <f t="shared" si="57"/>
-        <v>7280</v>
+        <v>10920</v>
       </c>
       <c r="O77" s="108">
         <f t="shared" si="57"/>
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="P77" s="109">
         <f t="shared" si="57"/>
@@ -20623,7 +20589,7 @@
       <c r="F78" s="215"/>
       <c r="G78" s="216">
         <f t="shared" ref="G78:H78" si="58">IF($Q$71 = "Choosing Supplier 1", SUM(H59:H60), SUM(H59:H60))</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H78" s="216">
         <f t="shared" si="58"/>
@@ -20639,15 +20605,15 @@
       </c>
       <c r="K78" s="216">
         <f t="shared" si="59"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L78" s="216">
         <f t="shared" si="59"/>
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="M78" s="216">
         <f t="shared" si="59"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N78" s="216">
         <f t="shared" si="59"/>
@@ -20727,7 +20693,7 @@
       </c>
       <c r="J79" s="79">
         <f t="shared" si="60"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K79" s="79">
         <f t="shared" si="60"/>
@@ -20739,7 +20705,7 @@
       </c>
       <c r="M79" s="79">
         <f t="shared" si="60"/>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="N79" s="79">
         <f t="shared" si="60"/>
@@ -20817,7 +20783,7 @@
       </c>
       <c r="J80" s="299">
         <f t="shared" si="61"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K80" s="299">
         <f t="shared" si="61"/>
@@ -20829,7 +20795,7 @@
       </c>
       <c r="M80" s="299">
         <f t="shared" si="61"/>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N80" s="299">
         <f t="shared" si="61"/>
@@ -20870,7 +20836,7 @@
       </c>
       <c r="J81" s="263">
         <f t="shared" si="62"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K81" s="263">
         <f t="shared" si="62"/>
@@ -20882,7 +20848,7 @@
       </c>
       <c r="M81" s="263">
         <f t="shared" si="62"/>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="N81" s="263">
         <f t="shared" si="62"/>
@@ -20941,7 +20907,7 @@
       </c>
       <c r="M82" s="83">
         <f t="shared" si="64"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N82" s="83">
         <f t="shared" si="64"/>
@@ -21024,7 +20990,7 @@
       </c>
       <c r="J83" s="83">
         <f t="shared" si="65"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K83" s="83">
         <f>IF($Q$71="Choosing Supplier 1", QUOTIENT(K81+$F$51-1,$F$50),QUOTIENT(K81+$F$53-1,$F$52))</f>
@@ -21036,7 +21002,7 @@
       </c>
       <c r="M83" s="83">
         <f t="shared" si="66"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N83" s="83">
         <f t="shared" si="66"/>
@@ -21116,7 +21082,7 @@
       </c>
       <c r="J84" s="130">
         <f t="shared" si="67"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K84" s="130">
         <f>IF($Q$71="Choosing Supplier 1", K83*$G$50+K82*$G$51, K83*$G$52+K82*$G$53)</f>
@@ -21128,7 +21094,7 @@
       </c>
       <c r="M84" s="130">
         <f t="shared" si="68"/>
-        <v>1280</v>
+        <v>500</v>
       </c>
       <c r="N84" s="130">
         <f t="shared" si="68"/>
@@ -21211,7 +21177,7 @@
       </c>
       <c r="J85" s="138">
         <f t="shared" si="69"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="K85" s="138">
         <f>K81*K72</f>
@@ -21223,7 +21189,7 @@
       </c>
       <c r="M85" s="138">
         <f t="shared" si="70"/>
-        <v>9630</v>
+        <v>3210</v>
       </c>
       <c r="N85" s="138">
         <f t="shared" si="70"/>
@@ -21304,7 +21270,7 @@
       </c>
       <c r="J86" s="108">
         <f t="shared" si="71"/>
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="K86" s="108">
         <f t="shared" si="71"/>
@@ -21316,7 +21282,7 @@
       </c>
       <c r="M86" s="108">
         <f t="shared" si="71"/>
-        <v>10910</v>
+        <v>3710</v>
       </c>
       <c r="N86" s="108">
         <f t="shared" si="71"/>
@@ -21354,7 +21320,7 @@
       </c>
       <c r="J87" s="138">
         <f t="shared" si="72"/>
-        <v>8260</v>
+        <v>0</v>
       </c>
       <c r="K87" s="138">
         <f>K81*K75</f>
@@ -21366,7 +21332,7 @@
       </c>
       <c r="M87" s="138">
         <f t="shared" si="73"/>
-        <v>19170</v>
+        <v>6390</v>
       </c>
       <c r="N87" s="138">
         <f t="shared" si="73"/>
@@ -21404,7 +21370,7 @@
       </c>
       <c r="J88" s="141">
         <f t="shared" si="74"/>
-        <v>3460</v>
+        <v>0</v>
       </c>
       <c r="K88" s="141">
         <f t="shared" si="74"/>
@@ -21416,7 +21382,7 @@
       </c>
       <c r="M88" s="141">
         <f t="shared" si="74"/>
-        <v>8260</v>
+        <v>2680</v>
       </c>
       <c r="N88" s="141">
         <f t="shared" si="74"/>
@@ -21445,7 +21411,7 @@
       <c r="F89" s="145"/>
       <c r="G89" s="146">
         <f>G77-G88</f>
-        <v>7040</v>
+        <v>3520</v>
       </c>
       <c r="H89" s="146">
         <f>H77-H88</f>
@@ -21457,7 +21423,7 @@
       </c>
       <c r="J89" s="146">
         <f t="shared" si="75"/>
-        <v>6920</v>
+        <v>13840</v>
       </c>
       <c r="K89" s="146">
         <f t="shared" si="75"/>
@@ -21465,19 +21431,19 @@
       </c>
       <c r="L89" s="146">
         <f t="shared" si="75"/>
-        <v>18700</v>
+        <v>11220</v>
       </c>
       <c r="M89" s="146">
         <f t="shared" si="75"/>
-        <v>10440</v>
+        <v>8540</v>
       </c>
       <c r="N89" s="146">
         <f t="shared" si="75"/>
-        <v>7280</v>
+        <v>10920</v>
       </c>
       <c r="O89" s="146">
         <f t="shared" si="75"/>
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="P89" s="147">
         <f t="shared" si="75"/>
@@ -21507,15 +21473,15 @@
       </c>
       <c r="J90" s="150">
         <f t="shared" si="76"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="K90" s="150">
         <f t="shared" si="76"/>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="L90" s="150">
         <f t="shared" si="76"/>
-        <v>0.6</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M90" s="150">
         <f t="shared" si="76"/>
@@ -21525,9 +21491,9 @@
         <f t="shared" si="76"/>
         <v>0</v>
       </c>
-      <c r="O90" s="150">
+      <c r="O90" s="150" t="e">
         <f t="shared" si="76"/>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P90" s="150" t="e">
         <f t="shared" si="76"/>
@@ -21554,7 +21520,7 @@
       </c>
       <c r="J91" s="150">
         <f t="shared" si="77"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K91" s="150">
         <f t="shared" si="77"/>
@@ -21566,15 +21532,15 @@
       </c>
       <c r="M91" s="150">
         <f t="shared" si="77"/>
-        <v>0.45648535564853554</v>
+        <v>0.25871687587168757</v>
       </c>
       <c r="N91" s="150">
         <f t="shared" si="77"/>
         <v>0</v>
       </c>
-      <c r="O91" s="150">
+      <c r="O91" s="150" t="e">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P91" s="150" t="e">
         <f t="shared" si="77"/>
@@ -21601,7 +21567,7 @@
       </c>
       <c r="J92" s="150">
         <f t="shared" si="78"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K92" s="150">
         <f t="shared" si="78"/>
@@ -21613,15 +21579,15 @@
       </c>
       <c r="M92" s="150">
         <f t="shared" si="78"/>
-        <v>0.44171122994652406</v>
+        <v>0.23885918003565063</v>
       </c>
       <c r="N92" s="150">
         <f t="shared" si="78"/>
         <v>0</v>
       </c>
-      <c r="O92" s="150">
+      <c r="O92" s="150" t="e">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P92" s="150" t="e">
         <f t="shared" si="78"/>
@@ -21841,7 +21807,7 @@
       </c>
       <c r="L105" s="65">
         <f>'DC3'!H13</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M105" s="65">
         <f>'DC3'!I13</f>
@@ -22025,7 +21991,7 @@
       </c>
       <c r="L109" s="207">
         <f t="shared" si="79"/>
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="M109" s="207">
         <f t="shared" si="79"/>
@@ -22145,7 +22111,7 @@
       </c>
       <c r="L112" s="68">
         <f t="shared" si="81"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M112" s="68">
         <f t="shared" si="81"/>
@@ -22194,7 +22160,7 @@
       </c>
       <c r="L113" s="175">
         <f t="shared" si="82"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M113" s="175">
         <f t="shared" si="82"/>
@@ -22240,7 +22206,7 @@
       </c>
       <c r="L114" s="75">
         <f t="shared" si="83"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M114" s="75">
         <f t="shared" si="83"/>
@@ -22333,7 +22299,7 @@
       </c>
       <c r="L116" s="83">
         <f t="shared" si="85"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M116" s="83">
         <f t="shared" si="85"/>
@@ -22379,7 +22345,7 @@
       </c>
       <c r="L117" s="87">
         <f t="shared" si="86"/>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="M117" s="87">
         <f t="shared" si="86"/>
@@ -22481,7 +22447,7 @@
       </c>
       <c r="L119" s="95">
         <f t="shared" si="87"/>
-        <v>3240</v>
+        <v>12960</v>
       </c>
       <c r="M119" s="95">
         <f t="shared" si="87"/>
@@ -22530,7 +22496,7 @@
       </c>
       <c r="L120" s="100">
         <f t="shared" si="88"/>
-        <v>3440</v>
+        <v>13560</v>
       </c>
       <c r="M120" s="100">
         <f t="shared" si="88"/>
@@ -22625,7 +22591,7 @@
       </c>
       <c r="L122" s="104">
         <f t="shared" si="89"/>
-        <v>6450</v>
+        <v>25800</v>
       </c>
       <c r="M122" s="104">
         <f t="shared" si="89"/>
@@ -22674,7 +22640,7 @@
       </c>
       <c r="L123" s="108">
         <f t="shared" si="90"/>
-        <v>3010</v>
+        <v>12240</v>
       </c>
       <c r="M123" s="108">
         <f t="shared" si="90"/>
@@ -22737,7 +22703,7 @@
       </c>
       <c r="L124" s="216">
         <f t="shared" si="91"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M124" s="216">
         <f t="shared" si="91"/>
@@ -22792,7 +22758,7 @@
       </c>
       <c r="J125" s="79">
         <f t="shared" si="92"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K125" s="79">
         <f t="shared" si="92"/>
@@ -22804,7 +22770,7 @@
       </c>
       <c r="M125" s="79">
         <f t="shared" si="92"/>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="N125" s="79">
         <f t="shared" si="92"/>
@@ -22853,7 +22819,7 @@
       </c>
       <c r="J126" s="299">
         <f t="shared" si="93"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K126" s="299">
         <f t="shared" si="93"/>
@@ -22865,7 +22831,7 @@
       </c>
       <c r="M126" s="299">
         <f t="shared" si="93"/>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="N126" s="299">
         <f t="shared" si="93"/>
@@ -22914,7 +22880,7 @@
       </c>
       <c r="J127" s="263">
         <f t="shared" si="94"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K127" s="263">
         <f t="shared" si="94"/>
@@ -22926,7 +22892,7 @@
       </c>
       <c r="M127" s="263">
         <f t="shared" si="94"/>
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N127" s="263">
         <f t="shared" si="94"/>
@@ -22995,7 +22961,7 @@
       </c>
       <c r="M128" s="83">
         <f t="shared" si="96"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N128" s="83">
         <f t="shared" si="96"/>
@@ -23049,7 +23015,7 @@
       </c>
       <c r="J129" s="83">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K129" s="83">
         <f>IF(Q117="Choosing Supplier 1", QUOTIENT(K127+$F$97-1,$F$96), QUOTIENT(K127+$F$99-1,$F$98))</f>
@@ -23061,7 +23027,7 @@
       </c>
       <c r="M129" s="83">
         <f t="shared" si="98"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N129" s="83">
         <f t="shared" si="98"/>
@@ -23112,7 +23078,7 @@
       </c>
       <c r="J130" s="130">
         <f t="shared" si="99"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="K130" s="130">
         <f t="shared" si="99"/>
@@ -23124,7 +23090,7 @@
       </c>
       <c r="M130" s="130">
         <f t="shared" ref="M130" si="100">IF($Q$117="Choosing Supplier 1", M129*$G$96+M128*$G$97, M129*$G$98+M128*$G$99)</f>
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="N130" s="130">
         <f t="shared" ref="N130" si="101">IF($Q$117="Choosing Supplier 1", N129*$G$96+N128*$G$97, N129*$G$98+N128*$G$99)</f>
@@ -23178,7 +23144,7 @@
       </c>
       <c r="J131" s="138">
         <f t="shared" si="104"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="K131" s="138">
         <f>K127*K118</f>
@@ -23190,7 +23156,7 @@
       </c>
       <c r="M131" s="138">
         <f t="shared" si="105"/>
-        <v>11770</v>
+        <v>5350</v>
       </c>
       <c r="N131" s="138">
         <f t="shared" si="105"/>
@@ -23242,7 +23208,7 @@
       </c>
       <c r="J132" s="108">
         <f t="shared" si="106"/>
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="K132" s="108">
         <f t="shared" si="106"/>
@@ -23254,7 +23220,7 @@
       </c>
       <c r="M132" s="108">
         <f t="shared" si="106"/>
-        <v>12370</v>
+        <v>5670</v>
       </c>
       <c r="N132" s="108">
         <f t="shared" si="106"/>
@@ -23305,7 +23271,7 @@
       </c>
       <c r="J133" s="138">
         <f t="shared" si="107"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="K133" s="138">
         <f>K127*K121</f>
@@ -23317,7 +23283,7 @@
       </c>
       <c r="M133" s="138">
         <f t="shared" si="108"/>
-        <v>23265</v>
+        <v>10575</v>
       </c>
       <c r="N133" s="138">
         <f t="shared" si="108"/>
@@ -23354,7 +23320,7 @@
       </c>
       <c r="J134" s="141">
         <f t="shared" si="109"/>
-        <v>3800</v>
+        <v>0</v>
       </c>
       <c r="K134" s="141">
         <f t="shared" si="109"/>
@@ -23366,7 +23332,7 @@
       </c>
       <c r="M134" s="141">
         <f t="shared" si="109"/>
-        <v>10895</v>
+        <v>4905</v>
       </c>
       <c r="N134" s="141">
         <f t="shared" si="109"/>
@@ -23406,7 +23372,7 @@
       </c>
       <c r="J135" s="146">
         <f t="shared" si="110"/>
-        <v>7600</v>
+        <v>11400</v>
       </c>
       <c r="K135" s="146">
         <f t="shared" si="110"/>
@@ -23414,11 +23380,11 @@
       </c>
       <c r="L135" s="146">
         <f t="shared" si="110"/>
-        <v>3010</v>
+        <v>12240</v>
       </c>
       <c r="M135" s="146">
         <f t="shared" si="110"/>
-        <v>15920</v>
+        <v>21910</v>
       </c>
       <c r="N135" s="146">
         <f t="shared" si="110"/>
@@ -23464,7 +23430,7 @@
       </c>
       <c r="L136" s="150">
         <f t="shared" si="111"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="M136" s="150">
         <f t="shared" si="111"/>
@@ -23503,7 +23469,7 @@
       </c>
       <c r="J137" s="150">
         <f t="shared" si="112"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K137" s="150">
         <f t="shared" si="112"/>
@@ -23515,7 +23481,7 @@
       </c>
       <c r="M137" s="150">
         <f t="shared" si="112"/>
-        <v>0.40838560581049854</v>
+        <v>0.18719049191152196</v>
       </c>
       <c r="N137" s="150">
         <f t="shared" si="112"/>
@@ -23550,7 +23516,7 @@
       </c>
       <c r="J138" s="150">
         <f t="shared" si="113"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="K138" s="150">
         <f t="shared" si="113"/>
@@ -23562,7 +23528,7 @@
       </c>
       <c r="M138" s="150">
         <f t="shared" si="113"/>
-        <v>0.40630244266268878</v>
+        <v>0.18292000745851203</v>
       </c>
       <c r="N138" s="150">
         <f t="shared" si="113"/>
@@ -23634,7 +23600,7 @@
       </c>
       <c r="F144" s="6">
         <f>Supplier1!C7</f>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G144" t="s">
         <v>35</v>
@@ -23667,7 +23633,7 @@
       </c>
       <c r="F146" s="7">
         <f>Supplier1!C4</f>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="O146" s="301"/>
       <c r="P146" s="301"/>
@@ -23732,23 +23698,23 @@
       </c>
       <c r="H149" s="282">
         <f t="shared" ref="H149:P149" si="114">IF($Q$26 = "Choosing Supplier 1", IF($F$147="Yes", H23,0),0)</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I149" s="282">
         <f t="shared" si="114"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="J149" s="282">
         <f t="shared" si="114"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K149" s="282">
         <f t="shared" si="114"/>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="L149" s="282">
         <f t="shared" si="114"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M149" s="282">
         <f t="shared" si="114"/>
@@ -23774,7 +23740,7 @@
       <c r="F150" s="271"/>
       <c r="G150" s="272">
         <f>IF($Q$71 = "Choosing Supplier 1", IF($F$147="Yes", G68,0),0)</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H150" s="272">
         <f t="shared" ref="H150:P150" si="115">IF($Q$71 = "Choosing Supplier 1", IF($F$147="Yes", H68,0),0)</f>
@@ -23786,7 +23752,7 @@
       </c>
       <c r="J150" s="272">
         <f t="shared" si="115"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K150" s="272">
         <f t="shared" si="115"/>
@@ -23794,19 +23760,19 @@
       </c>
       <c r="L150" s="272">
         <f t="shared" si="115"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="M150" s="272">
         <f t="shared" si="115"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N150" s="272">
         <f t="shared" si="115"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="O150" s="272">
         <f t="shared" si="115"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P150" s="273">
         <f t="shared" si="115"/>
@@ -23840,7 +23806,7 @@
       </c>
       <c r="L151" s="275">
         <f t="shared" si="116"/>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M151" s="275">
         <f t="shared" si="116"/>
@@ -23866,39 +23832,39 @@
       <c r="F152" s="186"/>
       <c r="G152" s="287">
         <f>SUM(G149:G151)</f>
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="H152" s="287">
         <f t="shared" ref="H152:P152" si="117">SUM(H149:H151)</f>
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="I152" s="287">
         <f t="shared" si="117"/>
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J152" s="287">
         <f t="shared" si="117"/>
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="K152" s="287">
         <f t="shared" si="117"/>
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="L152" s="287">
         <f t="shared" si="117"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="M152" s="287">
         <f t="shared" si="117"/>
-        <v>275</v>
+        <v>235</v>
       </c>
       <c r="N152" s="287">
         <f t="shared" si="117"/>
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O152" s="287">
         <f t="shared" si="117"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="P152" s="288">
         <f t="shared" si="117"/>
@@ -23931,7 +23897,7 @@
       </c>
       <c r="G154" s="68">
         <f t="shared" ref="G154:P154" si="118">F154+G156-G152</f>
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="H154" s="68">
         <f t="shared" si="118"/>
@@ -23939,35 +23905,35 @@
       </c>
       <c r="I154" s="68">
         <f t="shared" si="118"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J154" s="68">
         <f t="shared" si="118"/>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K154" s="68">
         <f t="shared" si="118"/>
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="L154" s="68">
         <f t="shared" si="118"/>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="M154" s="68">
         <f t="shared" si="118"/>
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="N154" s="68">
         <f t="shared" si="118"/>
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="O154" s="68">
         <f t="shared" si="118"/>
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="P154" s="69">
         <f t="shared" si="118"/>
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="155" spans="5:17" x14ac:dyDescent="0.3">
@@ -23977,7 +23943,7 @@
       <c r="F155" s="71"/>
       <c r="G155" s="68">
         <f t="shared" ref="G155:P155" si="119">IF(F154-G152&lt;=$F$145, G152-F154+$F$145,0)</f>
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="H155" s="68">
         <f t="shared" si="119"/>
@@ -23985,35 +23951,35 @@
       </c>
       <c r="I155" s="68">
         <f t="shared" si="119"/>
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="J155" s="68">
         <f t="shared" si="119"/>
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="K155" s="68">
         <f t="shared" si="119"/>
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="L155" s="68">
         <f t="shared" si="119"/>
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="M155" s="68">
         <f t="shared" si="119"/>
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="N155" s="68">
         <f t="shared" si="119"/>
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="O155" s="68">
         <f t="shared" si="119"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P155" s="69">
         <f t="shared" si="119"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="156" spans="5:17" x14ac:dyDescent="0.3">
@@ -24023,7 +23989,7 @@
       <c r="F156" s="71"/>
       <c r="G156" s="68">
         <f xml:space="preserve"> CEILING(G155/$F$144,1)*$F$144</f>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="H156" s="68">
         <f t="shared" ref="H156:P156" si="120" xml:space="preserve"> CEILING(H155/$F$144,1)*$F$144</f>
@@ -24031,35 +23997,35 @@
       </c>
       <c r="I156" s="68">
         <f t="shared" si="120"/>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="J156" s="68">
         <f t="shared" si="120"/>
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="K156" s="68">
         <f t="shared" si="120"/>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="L156" s="68">
         <f t="shared" si="120"/>
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="M156" s="68">
         <f t="shared" si="120"/>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="N156" s="68">
         <f t="shared" si="120"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="O156" s="68">
         <f t="shared" si="120"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="P156" s="69">
         <f t="shared" si="120"/>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="157" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -24073,35 +24039,35 @@
       </c>
       <c r="H157" s="195">
         <f>I156</f>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="I157" s="195">
         <f t="shared" ref="I157:P157" si="121">J156</f>
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="J157" s="195">
         <f t="shared" si="121"/>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="K157" s="195">
         <f t="shared" si="121"/>
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="L157" s="195">
         <f t="shared" si="121"/>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="M157" s="195">
         <f t="shared" si="121"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="N157" s="195">
         <f t="shared" si="121"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="O157" s="195">
         <f t="shared" si="121"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P157" s="196">
         <f t="shared" si="121"/>
@@ -24128,7 +24094,7 @@
       </c>
       <c r="J158" s="199">
         <f t="shared" si="122"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K158" s="199">
         <f>IF(K155&gt;$F$146,K155-$F$146,0)</f>
@@ -24140,7 +24106,7 @@
       </c>
       <c r="M158" s="199">
         <f t="shared" si="122"/>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="N158" s="199">
         <f t="shared" si="122"/>
@@ -24175,7 +24141,7 @@
       </c>
       <c r="J159" s="199">
         <f t="shared" si="122"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K159" s="199">
         <f t="shared" si="122"/>
@@ -24187,7 +24153,7 @@
       </c>
       <c r="M159" s="199">
         <f t="shared" si="122"/>
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="N159" s="199">
         <f t="shared" si="122"/>
@@ -24275,7 +24241,7 @@
       </c>
       <c r="F167" s="7">
         <f>Supplier2!C4</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="O167" s="301"/>
       <c r="P167" s="301"/>
@@ -24920,7 +24886,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>